<commit_message>
UO Outlands Creature List.v01
</commit_message>
<xml_diff>
--- a/UO Outlands Creature List.xlsx
+++ b/UO Outlands Creature List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeff\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BE591B9-AC6F-4400-8E22-FF53B00CCD13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDF49CF2-3041-42EB-9457-8CA1188C6E9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31110" yWindow="2865" windowWidth="21600" windowHeight="11385" xr2:uid="{725F3C2E-E349-4B8F-BF20-9916B673D670}"/>
+    <workbookView xWindow="37440" yWindow="1920" windowWidth="21600" windowHeight="11385" xr2:uid="{725F3C2E-E349-4B8F-BF20-9916B673D670}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 0" sheetId="2" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1691" uniqueCount="888">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1795" uniqueCount="990">
   <si>
     <t>Slayer</t>
   </si>
@@ -2712,6 +2712,312 @@
   </si>
   <si>
     <t>0x7C647</t>
+  </si>
+  <si>
+    <t>a gremlin</t>
+  </si>
+  <si>
+    <t>0x1B9C6</t>
+  </si>
+  <si>
+    <t>a goblin</t>
+  </si>
+  <si>
+    <t>0x1B9B4</t>
+  </si>
+  <si>
+    <t>an aegis mongbat</t>
+  </si>
+  <si>
+    <t>0x1A11C</t>
+  </si>
+  <si>
+    <t>an effigy</t>
+  </si>
+  <si>
+    <t>0x1A0E0</t>
+  </si>
+  <si>
+    <t>an aegis rat</t>
+  </si>
+  <si>
+    <t>0x1A05C</t>
+  </si>
+  <si>
+    <t>an aegis cultist</t>
+  </si>
+  <si>
+    <t>0x2432BE</t>
+  </si>
+  <si>
+    <t>an entombed</t>
+  </si>
+  <si>
+    <t>0x2432A3</t>
+  </si>
+  <si>
+    <t>an aegis slime</t>
+  </si>
+  <si>
+    <t>0x1B9CC</t>
+  </si>
+  <si>
+    <t>a wolfhound</t>
+  </si>
+  <si>
+    <t>0x1A0E6</t>
+  </si>
+  <si>
+    <t>a kobold</t>
+  </si>
+  <si>
+    <t>0x1A052</t>
+  </si>
+  <si>
+    <t>a chaos footman</t>
+  </si>
+  <si>
+    <t>0x1B9C4</t>
+  </si>
+  <si>
+    <t>an aegis imp</t>
+  </si>
+  <si>
+    <t>0x1B9D3</t>
+  </si>
+  <si>
+    <t>a blood ape</t>
+  </si>
+  <si>
+    <t>0x1A0F6</t>
+  </si>
+  <si>
+    <t>an aegis minion</t>
+  </si>
+  <si>
+    <t>0x1A079</t>
+  </si>
+  <si>
+    <t>a blood hellion</t>
+  </si>
+  <si>
+    <t>0x1B9FD</t>
+  </si>
+  <si>
+    <t>a blood orc</t>
+  </si>
+  <si>
+    <t>0x1B9EC</t>
+  </si>
+  <si>
+    <t>an aegis whelp</t>
+  </si>
+  <si>
+    <t>0x18645</t>
+  </si>
+  <si>
+    <t>a blood ogre mage</t>
+  </si>
+  <si>
+    <t>0x12AB9</t>
+  </si>
+  <si>
+    <t>a blood troll</t>
+  </si>
+  <si>
+    <t>0x12AAD</t>
+  </si>
+  <si>
+    <t>a clay man</t>
+  </si>
+  <si>
+    <t>0x12AAF</t>
+  </si>
+  <si>
+    <t>a blood harpy</t>
+  </si>
+  <si>
+    <t>0xC360</t>
+  </si>
+  <si>
+    <t>a blood drake</t>
+  </si>
+  <si>
+    <t>0x10303</t>
+  </si>
+  <si>
+    <t>an aegis noble</t>
+  </si>
+  <si>
+    <t>0x10305</t>
+  </si>
+  <si>
+    <t>an aegis asp</t>
+  </si>
+  <si>
+    <t>0x10356</t>
+  </si>
+  <si>
+    <t>an aegis scorpion</t>
+  </si>
+  <si>
+    <t>0xE58B</t>
+  </si>
+  <si>
+    <t>an aegis lich</t>
+  </si>
+  <si>
+    <t>0xE58C</t>
+  </si>
+  <si>
+    <t>a bloodrat</t>
+  </si>
+  <si>
+    <t>0x18647</t>
+  </si>
+  <si>
+    <t>a coagulator</t>
+  </si>
+  <si>
+    <t>0x12ABB</t>
+  </si>
+  <si>
+    <t>an aegis leech</t>
+  </si>
+  <si>
+    <t>0x1111A</t>
+  </si>
+  <si>
+    <t>a twilight guardian</t>
+  </si>
+  <si>
+    <t>0x1112B</t>
+  </si>
+  <si>
+    <t>a skulker</t>
+  </si>
+  <si>
+    <t>0x12ABC</t>
+  </si>
+  <si>
+    <t>a bloodwolf</t>
+  </si>
+  <si>
+    <t>0x107F9</t>
+  </si>
+  <si>
+    <t>a chaos warrior</t>
+  </si>
+  <si>
+    <t>0x255984</t>
+  </si>
+  <si>
+    <t>a blood cyclops</t>
+  </si>
+  <si>
+    <t>0x25596A</t>
+  </si>
+  <si>
+    <t>an aegis knight</t>
+  </si>
+  <si>
+    <t>0x25583F</t>
+  </si>
+  <si>
+    <t>a malform</t>
+  </si>
+  <si>
+    <t>0x1BA19</t>
+  </si>
+  <si>
+    <t>a blood scorpion</t>
+  </si>
+  <si>
+    <t>0x1BA18</t>
+  </si>
+  <si>
+    <t>a chaos knight</t>
+  </si>
+  <si>
+    <t>0x1BA24</t>
+  </si>
+  <si>
+    <t>a blood serpent</t>
+  </si>
+  <si>
+    <t>0x16B22</t>
+  </si>
+  <si>
+    <t>a doppelganger</t>
+  </si>
+  <si>
+    <t>0x163E0</t>
+  </si>
+  <si>
+    <t>a blood ravager</t>
+  </si>
+  <si>
+    <t>0x18649</t>
+  </si>
+  <si>
+    <t>blood elemental</t>
+  </si>
+  <si>
+    <t>0xF78C</t>
+  </si>
+  <si>
+    <t>a blood fiend</t>
+  </si>
+  <si>
+    <t>0x103BF</t>
+  </si>
+  <si>
+    <t>a lesser blood daemon</t>
+  </si>
+  <si>
+    <t>0x103F7</t>
+  </si>
+  <si>
+    <t>a bloodworm</t>
+  </si>
+  <si>
+    <t>0x103FD</t>
+  </si>
+  <si>
+    <t>a blood dragon</t>
+  </si>
+  <si>
+    <t>0x17EFF</t>
+  </si>
+  <si>
+    <t>a blood feaster</t>
+  </si>
+  <si>
+    <t>0x101A5</t>
+  </si>
+  <si>
+    <t>a blood hunter</t>
+  </si>
+  <si>
+    <t>0x17EF9</t>
+  </si>
+  <si>
+    <t>a blood sorcerer</t>
+  </si>
+  <si>
+    <t>0x17F09</t>
+  </si>
+  <si>
+    <t>a blood daemon</t>
+  </si>
+  <si>
+    <t>0x1BDD6</t>
+  </si>
+  <si>
+    <t>0x100B0</t>
+  </si>
+  <si>
+    <t>0x1B8A9</t>
   </si>
 </sst>
 </file>
@@ -3214,8 +3520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B23D4693-46C3-4AB6-951E-1D31349F3F3F}">
   <dimension ref="A1:V734"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A581" workbookViewId="0">
-      <selection activeCell="D592" sqref="D592"/>
+    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="D76" sqref="D76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3524,10 +3830,18 @@
       <c r="V6" s="2"/>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
+      <c r="A7" s="2" t="s">
+        <v>934</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>935</v>
+      </c>
+      <c r="C7" s="2">
+        <v>2853</v>
+      </c>
+      <c r="D7" s="2">
+        <v>727</v>
+      </c>
       <c r="E7" s="2" t="s">
         <v>27</v>
       </c>
@@ -3567,10 +3881,18 @@
       <c r="V7" s="2"/>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
+      <c r="A8" s="2" t="s">
+        <v>898</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>899</v>
+      </c>
+      <c r="C8" s="2">
+        <v>2928</v>
+      </c>
+      <c r="D8" s="2">
+        <v>689</v>
+      </c>
       <c r="E8" s="2" t="s">
         <v>28</v>
       </c>
@@ -3654,10 +3976,18 @@
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
+      <c r="A10" s="2" t="s">
+        <v>910</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>911</v>
+      </c>
+      <c r="C10" s="2">
+        <v>2853</v>
+      </c>
+      <c r="D10" s="2">
+        <v>74</v>
+      </c>
       <c r="E10" s="2" t="s">
         <v>31</v>
       </c>
@@ -3701,10 +4031,18 @@
       <c r="V10" s="2"/>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
+      <c r="A11" s="2" t="s">
+        <v>956</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>957</v>
+      </c>
+      <c r="C11" s="2">
+        <v>1055</v>
+      </c>
+      <c r="D11" s="2">
+        <v>400</v>
+      </c>
       <c r="E11" s="2" t="s">
         <v>32</v>
       </c>
@@ -3742,10 +4080,18 @@
       <c r="V11" s="2"/>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
+      <c r="A12" s="2" t="s">
+        <v>944</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>945</v>
+      </c>
+      <c r="C12" s="2">
+        <v>2944</v>
+      </c>
+      <c r="D12" s="2">
+        <v>732</v>
+      </c>
       <c r="E12" s="2" t="s">
         <v>33</v>
       </c>
@@ -3780,10 +4126,18 @@
       <c r="V12" s="2"/>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
+      <c r="A13" s="2" t="s">
+        <v>938</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>939</v>
+      </c>
+      <c r="C13" s="2">
+        <v>2944</v>
+      </c>
+      <c r="D13" s="2">
+        <v>24</v>
+      </c>
       <c r="E13" s="2" t="s">
         <v>35</v>
       </c>
@@ -3827,10 +4181,18 @@
       <c r="V13" s="2"/>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
+      <c r="A14" s="2" t="s">
+        <v>914</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>915</v>
+      </c>
+      <c r="C14" s="2">
+        <v>2928</v>
+      </c>
+      <c r="D14" s="2">
+        <v>776</v>
+      </c>
       <c r="E14" s="2" t="s">
         <v>37</v>
       </c>
@@ -3874,10 +4236,18 @@
       <c r="V14" s="2"/>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
+      <c r="A15" s="2" t="s">
+        <v>892</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>893</v>
+      </c>
+      <c r="C15" s="2">
+        <v>2819</v>
+      </c>
+      <c r="D15" s="2">
+        <v>39</v>
+      </c>
       <c r="E15" s="2" t="s">
         <v>38</v>
       </c>
@@ -3912,10 +4282,18 @@
       <c r="V15" s="2"/>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
+      <c r="A16" s="2" t="s">
+        <v>932</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>933</v>
+      </c>
+      <c r="C16" s="2">
+        <v>1048</v>
+      </c>
+      <c r="D16" s="2">
+        <v>400</v>
+      </c>
       <c r="E16" s="2" t="s">
         <v>39</v>
       </c>
@@ -3950,10 +4328,18 @@
       <c r="V16" s="2"/>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
+      <c r="A17" s="2" t="s">
+        <v>896</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>897</v>
+      </c>
+      <c r="C17" s="2">
+        <v>2944</v>
+      </c>
+      <c r="D17" s="2">
+        <v>215</v>
+      </c>
       <c r="E17" s="2" t="s">
         <v>40</v>
       </c>
@@ -3988,10 +4374,18 @@
       <c r="V17" s="2"/>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
+      <c r="A18" s="2" t="s">
+        <v>936</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>937</v>
+      </c>
+      <c r="C18" s="2">
+        <v>2944</v>
+      </c>
+      <c r="D18" s="2">
+        <v>717</v>
+      </c>
       <c r="E18" s="2" t="s">
         <v>41</v>
       </c>
@@ -4031,10 +4425,18 @@
       <c r="V18" s="2"/>
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
+      <c r="A19" s="2" t="s">
+        <v>902</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>903</v>
+      </c>
+      <c r="C19" s="2">
+        <v>2944</v>
+      </c>
+      <c r="D19" s="2">
+        <v>51</v>
+      </c>
       <c r="E19" s="2" t="s">
         <v>42</v>
       </c>
@@ -4072,10 +4474,18 @@
       <c r="V19" s="2"/>
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
+      <c r="A20" s="2" t="s">
+        <v>920</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>921</v>
+      </c>
+      <c r="C20" s="2">
+        <v>2853</v>
+      </c>
+      <c r="D20" s="2">
+        <v>716</v>
+      </c>
       <c r="E20" s="2" t="s">
         <v>44</v>
       </c>
@@ -6025,10 +6435,18 @@
       <c r="V65" s="2"/>
     </row>
     <row r="66" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A66" s="2"/>
-      <c r="B66" s="2"/>
-      <c r="C66" s="2"/>
-      <c r="D66" s="2"/>
+      <c r="A66" s="2" t="s">
+        <v>912</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>913</v>
+      </c>
+      <c r="C66" s="2">
+        <v>2466</v>
+      </c>
+      <c r="D66" s="2">
+        <v>29</v>
+      </c>
       <c r="E66" s="2" t="s">
         <v>92</v>
       </c>
@@ -6359,10 +6777,18 @@
       <c r="V73" s="2"/>
     </row>
     <row r="74" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A74" s="2"/>
-      <c r="B74" s="2"/>
-      <c r="C74" s="2"/>
-      <c r="D74" s="2"/>
+      <c r="A74" s="2" t="s">
+        <v>954</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>955</v>
+      </c>
+      <c r="C74" s="2">
+        <v>2740</v>
+      </c>
+      <c r="D74" s="2">
+        <v>75</v>
+      </c>
       <c r="E74" s="2" t="s">
         <v>100</v>
       </c>
@@ -6397,10 +6823,18 @@
       <c r="V74" s="2"/>
     </row>
     <row r="75" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A75" s="2"/>
-      <c r="B75" s="2"/>
-      <c r="C75" s="2"/>
-      <c r="D75" s="2"/>
+      <c r="A75" s="2" t="s">
+        <v>986</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>987</v>
+      </c>
+      <c r="C75" s="2">
+        <v>2740</v>
+      </c>
+      <c r="D75" s="2">
+        <v>9</v>
+      </c>
       <c r="E75" s="2" t="s">
         <v>101</v>
       </c>
@@ -6444,10 +6878,18 @@
       <c r="V75" s="2"/>
     </row>
     <row r="76" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A76" s="2"/>
-      <c r="B76" s="2"/>
-      <c r="C76" s="2"/>
-      <c r="D76" s="2"/>
+      <c r="A76" s="2" t="s">
+        <v>978</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>989</v>
+      </c>
+      <c r="C76" s="2">
+        <v>2740</v>
+      </c>
+      <c r="D76" s="2">
+        <v>59</v>
+      </c>
       <c r="E76" s="2" t="s">
         <v>102</v>
       </c>
@@ -6482,10 +6924,18 @@
       <c r="V76" s="2"/>
     </row>
     <row r="77" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A77" s="2"/>
-      <c r="B77" s="2"/>
-      <c r="C77" s="2"/>
-      <c r="D77" s="2"/>
+      <c r="A77" s="2" t="s">
+        <v>930</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>931</v>
+      </c>
+      <c r="C77" s="2">
+        <v>2740</v>
+      </c>
+      <c r="D77" s="2">
+        <v>61</v>
+      </c>
       <c r="E77" s="2" t="s">
         <v>103</v>
       </c>
@@ -6520,10 +6970,18 @@
       <c r="V77" s="2"/>
     </row>
     <row r="78" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A78" s="2"/>
-      <c r="B78" s="2"/>
-      <c r="C78" s="2"/>
-      <c r="D78" s="2"/>
+      <c r="A78" s="2" t="s">
+        <v>970</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>971</v>
+      </c>
+      <c r="C78" s="2">
+        <v>2846</v>
+      </c>
+      <c r="D78" s="2">
+        <v>16</v>
+      </c>
       <c r="E78" s="2" t="s">
         <v>104</v>
       </c>
@@ -6570,10 +7028,18 @@
       <c r="V78" s="2"/>
     </row>
     <row r="79" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A79" s="2"/>
-      <c r="B79" s="2"/>
-      <c r="C79" s="2"/>
-      <c r="D79" s="2"/>
+      <c r="A79" s="2" t="s">
+        <v>980</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>981</v>
+      </c>
+      <c r="C79" s="2">
+        <v>2740</v>
+      </c>
+      <c r="D79" s="2">
+        <v>303</v>
+      </c>
       <c r="E79" s="2" t="s">
         <v>105</v>
       </c>
@@ -6608,10 +7074,18 @@
       <c r="V79" s="2"/>
     </row>
     <row r="80" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A80" s="2"/>
-      <c r="B80" s="2"/>
-      <c r="C80" s="2"/>
-      <c r="D80" s="2"/>
+      <c r="A80" s="2" t="s">
+        <v>972</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>973</v>
+      </c>
+      <c r="C80" s="2">
+        <v>2740</v>
+      </c>
+      <c r="D80" s="2">
+        <v>306</v>
+      </c>
       <c r="E80" s="2" t="s">
         <v>106</v>
       </c>
@@ -6646,10 +7120,18 @@
       <c r="V80" s="2"/>
     </row>
     <row r="81" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A81" s="2"/>
-      <c r="B81" s="2"/>
-      <c r="C81" s="2"/>
-      <c r="D81" s="2"/>
+      <c r="A81" s="2" t="s">
+        <v>928</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>929</v>
+      </c>
+      <c r="C81" s="2">
+        <v>2740</v>
+      </c>
+      <c r="D81" s="2">
+        <v>30</v>
+      </c>
       <c r="E81" s="2" t="s">
         <v>107</v>
       </c>
@@ -6684,10 +7166,18 @@
       <c r="V81" s="2"/>
     </row>
     <row r="82" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A82" s="2"/>
-      <c r="B82" s="2"/>
-      <c r="C82" s="2"/>
-      <c r="D82" s="2"/>
+      <c r="A82" s="2" t="s">
+        <v>916</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>917</v>
+      </c>
+      <c r="C82" s="2">
+        <v>2740</v>
+      </c>
+      <c r="D82" s="2">
+        <v>241</v>
+      </c>
       <c r="E82" s="2" t="s">
         <v>108</v>
       </c>
@@ -6722,10 +7212,18 @@
       <c r="V82" s="2"/>
     </row>
     <row r="83" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A83" s="2"/>
-      <c r="B83" s="2"/>
-      <c r="C83" s="2"/>
-      <c r="D83" s="2"/>
+      <c r="A83" s="2" t="s">
+        <v>982</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>983</v>
+      </c>
+      <c r="C83" s="2">
+        <v>2817</v>
+      </c>
+      <c r="D83" s="2">
+        <v>730</v>
+      </c>
       <c r="E83" s="2" t="s">
         <v>109</v>
       </c>
@@ -6807,10 +7305,18 @@
       <c r="V84" s="2"/>
     </row>
     <row r="85" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A85" s="2"/>
-      <c r="B85" s="2"/>
-      <c r="C85" s="2"/>
-      <c r="D85" s="2"/>
+      <c r="A85" s="2" t="s">
+        <v>922</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>923</v>
+      </c>
+      <c r="C85" s="2">
+        <v>2846</v>
+      </c>
+      <c r="D85" s="2">
+        <v>1</v>
+      </c>
       <c r="E85" s="2" t="s">
         <v>111</v>
       </c>
@@ -6854,10 +7360,18 @@
       <c r="V85" s="2"/>
     </row>
     <row r="86" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A86" s="2"/>
-      <c r="B86" s="2"/>
-      <c r="C86" s="2"/>
-      <c r="D86" s="2"/>
+      <c r="A86" s="2" t="s">
+        <v>918</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>919</v>
+      </c>
+      <c r="C86" s="2">
+        <v>2740</v>
+      </c>
+      <c r="D86" s="2">
+        <v>17</v>
+      </c>
       <c r="E86" s="2" t="s">
         <v>112</v>
       </c>
@@ -6892,10 +7406,18 @@
       <c r="V86" s="2"/>
     </row>
     <row r="87" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A87" s="2"/>
-      <c r="B87" s="2"/>
-      <c r="C87" s="2"/>
-      <c r="D87" s="2"/>
+      <c r="A87" s="2" t="s">
+        <v>968</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>969</v>
+      </c>
+      <c r="C87" s="2">
+        <v>2740</v>
+      </c>
+      <c r="D87" s="2">
+        <v>314</v>
+      </c>
       <c r="E87" s="2" t="s">
         <v>113</v>
       </c>
@@ -6930,10 +7452,18 @@
       <c r="V87" s="2"/>
     </row>
     <row r="88" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A88" s="2"/>
-      <c r="B88" s="2"/>
-      <c r="C88" s="2"/>
-      <c r="D88" s="2"/>
+      <c r="A88" s="2" t="s">
+        <v>960</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>961</v>
+      </c>
+      <c r="C88" s="2">
+        <v>2466</v>
+      </c>
+      <c r="D88" s="2">
+        <v>48</v>
+      </c>
       <c r="E88" s="2" t="s">
         <v>114</v>
       </c>
@@ -6973,10 +7503,18 @@
       <c r="V88" s="2"/>
     </row>
     <row r="89" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A89" s="2"/>
-      <c r="B89" s="2"/>
-      <c r="C89" s="2"/>
-      <c r="D89" s="2"/>
+      <c r="A89" s="2" t="s">
+        <v>964</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>965</v>
+      </c>
+      <c r="C89" s="2">
+        <v>2846</v>
+      </c>
+      <c r="D89" s="2">
+        <v>21</v>
+      </c>
       <c r="E89" s="2" t="s">
         <v>115</v>
       </c>
@@ -7016,10 +7554,18 @@
       <c r="V89" s="2"/>
     </row>
     <row r="90" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A90" s="2"/>
-      <c r="B90" s="2"/>
-      <c r="C90" s="2"/>
-      <c r="D90" s="2"/>
+      <c r="A90" s="2" t="s">
+        <v>984</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>985</v>
+      </c>
+      <c r="C90" s="2">
+        <v>2740</v>
+      </c>
+      <c r="D90" s="2">
+        <v>721</v>
+      </c>
       <c r="E90" s="2" t="s">
         <v>116</v>
       </c>
@@ -7063,10 +7609,18 @@
       <c r="V90" s="2"/>
     </row>
     <row r="91" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A91" s="2"/>
-      <c r="B91" s="2"/>
-      <c r="C91" s="2"/>
-      <c r="D91" s="2"/>
+      <c r="A91" s="2" t="s">
+        <v>924</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>925</v>
+      </c>
+      <c r="C91" s="2">
+        <v>2846</v>
+      </c>
+      <c r="D91" s="2">
+        <v>53</v>
+      </c>
       <c r="E91" s="2" t="s">
         <v>117</v>
       </c>
@@ -7101,10 +7655,18 @@
       <c r="V91" s="2"/>
     </row>
     <row r="92" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A92" s="2"/>
-      <c r="B92" s="2"/>
-      <c r="C92" s="2"/>
-      <c r="D92" s="2"/>
+      <c r="A92" s="2" t="s">
+        <v>940</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>941</v>
+      </c>
+      <c r="C92" s="2">
+        <v>2466</v>
+      </c>
+      <c r="D92" s="2">
+        <v>42</v>
+      </c>
       <c r="E92" s="2" t="s">
         <v>118</v>
       </c>
@@ -7139,10 +7701,18 @@
       <c r="V92" s="2"/>
     </row>
     <row r="93" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A93" s="2"/>
-      <c r="B93" s="2"/>
-      <c r="C93" s="2"/>
-      <c r="D93" s="2"/>
+      <c r="A93" s="2" t="s">
+        <v>950</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>951</v>
+      </c>
+      <c r="C93" s="2">
+        <v>2740</v>
+      </c>
+      <c r="D93" s="2">
+        <v>1069</v>
+      </c>
       <c r="E93" s="2" t="s">
         <v>119</v>
       </c>
@@ -7177,10 +7747,18 @@
       <c r="V93" s="2"/>
     </row>
     <row r="94" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A94" s="2"/>
-      <c r="B94" s="2"/>
-      <c r="C94" s="2"/>
-      <c r="D94" s="2"/>
+      <c r="A94" s="2" t="s">
+        <v>976</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>977</v>
+      </c>
+      <c r="C94" s="2">
+        <v>2817</v>
+      </c>
+      <c r="D94" s="2">
+        <v>287</v>
+      </c>
       <c r="E94" s="2" t="s">
         <v>120</v>
       </c>
@@ -7215,10 +7793,18 @@
       <c r="V94" s="2"/>
     </row>
     <row r="95" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A95" s="2"/>
-      <c r="B95" s="2"/>
-      <c r="C95" s="2"/>
-      <c r="D95" s="2"/>
+      <c r="A95" s="2" t="s">
+        <v>978</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>979</v>
+      </c>
+      <c r="C95" s="2">
+        <v>2740</v>
+      </c>
+      <c r="D95" s="2">
+        <v>59</v>
+      </c>
       <c r="E95" s="2" t="s">
         <v>121</v>
       </c>
@@ -8390,10 +8976,18 @@
       <c r="V122" s="2"/>
     </row>
     <row r="123" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A123" s="2"/>
-      <c r="B123" s="2"/>
-      <c r="C123" s="2"/>
-      <c r="D123" s="2"/>
+      <c r="A123" s="2" t="s">
+        <v>908</v>
+      </c>
+      <c r="B123" s="2" t="s">
+        <v>909</v>
+      </c>
+      <c r="C123" s="2">
+        <v>0</v>
+      </c>
+      <c r="D123" s="2">
+        <v>23</v>
+      </c>
       <c r="E123" s="2" t="s">
         <v>149</v>
       </c>
@@ -8428,10 +9022,18 @@
       <c r="V123" s="2"/>
     </row>
     <row r="124" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A124" s="2"/>
-      <c r="B124" s="2"/>
-      <c r="C124" s="2"/>
-      <c r="D124" s="2"/>
+      <c r="A124" s="2" t="s">
+        <v>962</v>
+      </c>
+      <c r="B124" s="2" t="s">
+        <v>963</v>
+      </c>
+      <c r="C124" s="2">
+        <v>0</v>
+      </c>
+      <c r="D124" s="2">
+        <v>27</v>
+      </c>
       <c r="E124" s="2" t="s">
         <v>150</v>
       </c>
@@ -8466,10 +9068,18 @@
       <c r="V124" s="2"/>
     </row>
     <row r="125" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A125" s="2"/>
-      <c r="B125" s="2"/>
-      <c r="C125" s="2"/>
-      <c r="D125" s="2"/>
+      <c r="A125" s="2" t="s">
+        <v>952</v>
+      </c>
+      <c r="B125" s="2" t="s">
+        <v>953</v>
+      </c>
+      <c r="C125" s="2">
+        <v>0</v>
+      </c>
+      <c r="D125" s="2">
+        <v>25</v>
+      </c>
       <c r="E125" s="2" t="s">
         <v>151</v>
       </c>
@@ -8668,10 +9278,18 @@
       <c r="V129" s="2"/>
     </row>
     <row r="130" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A130" s="2"/>
-      <c r="B130" s="2"/>
-      <c r="C130" s="2"/>
-      <c r="D130" s="2"/>
+      <c r="A130" s="2" t="s">
+        <v>926</v>
+      </c>
+      <c r="B130" s="2" t="s">
+        <v>927</v>
+      </c>
+      <c r="C130" s="2">
+        <v>2798</v>
+      </c>
+      <c r="D130" s="2">
+        <v>779</v>
+      </c>
       <c r="E130" s="2" t="s">
         <v>156</v>
       </c>
@@ -8706,10 +9324,18 @@
       <c r="V130" s="2"/>
     </row>
     <row r="131" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A131" s="2"/>
-      <c r="B131" s="2"/>
-      <c r="C131" s="2"/>
-      <c r="D131" s="2"/>
+      <c r="A131" s="2" t="s">
+        <v>942</v>
+      </c>
+      <c r="B131" s="2" t="s">
+        <v>943</v>
+      </c>
+      <c r="C131" s="2">
+        <v>2740</v>
+      </c>
+      <c r="D131" s="2">
+        <v>775</v>
+      </c>
       <c r="E131" s="2" t="s">
         <v>157</v>
       </c>
@@ -10935,10 +11561,18 @@
       <c r="V184" s="2"/>
     </row>
     <row r="185" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A185" s="2"/>
-      <c r="B185" s="2"/>
-      <c r="C185" s="2"/>
-      <c r="D185" s="2"/>
+      <c r="A185" s="2" t="s">
+        <v>966</v>
+      </c>
+      <c r="B185" s="2" t="s">
+        <v>967</v>
+      </c>
+      <c r="C185" s="2">
+        <v>2479</v>
+      </c>
+      <c r="D185" s="2">
+        <v>777</v>
+      </c>
       <c r="E185" s="2" t="s">
         <v>210</v>
       </c>
@@ -12212,10 +12846,18 @@
       <c r="V214" s="2"/>
     </row>
     <row r="215" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A215" s="2"/>
-      <c r="B215" s="2"/>
-      <c r="C215" s="2"/>
-      <c r="D215" s="2"/>
+      <c r="A215" s="2" t="s">
+        <v>894</v>
+      </c>
+      <c r="B215" s="2" t="s">
+        <v>895</v>
+      </c>
+      <c r="C215" s="2">
+        <v>2910</v>
+      </c>
+      <c r="D215" s="2">
+        <v>31</v>
+      </c>
       <c r="E215" s="2" t="s">
         <v>240</v>
       </c>
@@ -12713,10 +13355,18 @@
       <c r="V226" s="2"/>
     </row>
     <row r="227" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A227" s="2"/>
-      <c r="B227" s="2"/>
-      <c r="C227" s="2"/>
-      <c r="D227" s="2"/>
+      <c r="A227" s="2" t="s">
+        <v>900</v>
+      </c>
+      <c r="B227" s="2" t="s">
+        <v>901</v>
+      </c>
+      <c r="C227" s="2">
+        <v>2797</v>
+      </c>
+      <c r="D227" s="2">
+        <v>154</v>
+      </c>
       <c r="E227" s="2" t="s">
         <v>252</v>
       </c>
@@ -15862,10 +16512,18 @@
       <c r="V299" s="2"/>
     </row>
     <row r="300" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A300" s="2"/>
-      <c r="B300" s="2"/>
-      <c r="C300" s="2"/>
-      <c r="D300" s="2"/>
+      <c r="A300" s="2" t="s">
+        <v>890</v>
+      </c>
+      <c r="B300" s="2" t="s">
+        <v>891</v>
+      </c>
+      <c r="C300" s="2">
+        <v>0</v>
+      </c>
+      <c r="D300" s="2">
+        <v>723</v>
+      </c>
       <c r="E300" s="2" t="s">
         <v>325</v>
       </c>
@@ -16186,10 +16844,18 @@
       <c r="V307" s="2"/>
     </row>
     <row r="308" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A308" s="2"/>
-      <c r="B308" s="2"/>
-      <c r="C308" s="2"/>
-      <c r="D308" s="2"/>
+      <c r="A308" s="2" t="s">
+        <v>888</v>
+      </c>
+      <c r="B308" s="2" t="s">
+        <v>889</v>
+      </c>
+      <c r="C308" s="2">
+        <v>2941</v>
+      </c>
+      <c r="D308" s="2">
+        <v>334</v>
+      </c>
       <c r="E308" s="2" t="s">
         <v>333</v>
       </c>
@@ -18103,10 +18769,18 @@
       <c r="V353" s="2"/>
     </row>
     <row r="354" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A354" s="2"/>
-      <c r="B354" s="2"/>
-      <c r="C354" s="2"/>
-      <c r="D354" s="2"/>
+      <c r="A354" s="2" t="s">
+        <v>906</v>
+      </c>
+      <c r="B354" s="2" t="s">
+        <v>907</v>
+      </c>
+      <c r="C354" s="2">
+        <v>0</v>
+      </c>
+      <c r="D354" s="2">
+        <v>724</v>
+      </c>
       <c r="E354" s="2" t="s">
         <v>379</v>
       </c>
@@ -18305,10 +18979,18 @@
       <c r="V358" s="2"/>
     </row>
     <row r="359" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A359" s="2"/>
-      <c r="B359" s="2"/>
-      <c r="C359" s="2"/>
-      <c r="D359" s="2"/>
+      <c r="A359" s="2" t="s">
+        <v>974</v>
+      </c>
+      <c r="B359" s="2" t="s">
+        <v>975</v>
+      </c>
+      <c r="C359" s="2">
+        <v>2740</v>
+      </c>
+      <c r="D359" s="2">
+        <v>40</v>
+      </c>
       <c r="E359" s="2" t="s">
         <v>384</v>
       </c>
@@ -19450,10 +20132,18 @@
       <c r="V384" s="2"/>
     </row>
     <row r="385" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A385" s="2"/>
-      <c r="B385" s="2"/>
-      <c r="C385" s="2"/>
-      <c r="D385" s="2"/>
+      <c r="A385" s="2" t="s">
+        <v>958</v>
+      </c>
+      <c r="B385" s="2" t="s">
+        <v>959</v>
+      </c>
+      <c r="C385" s="2">
+        <v>2846</v>
+      </c>
+      <c r="D385" s="2">
+        <v>259</v>
+      </c>
       <c r="E385" s="2" t="s">
         <v>410</v>
       </c>
@@ -27243,10 +27933,18 @@
       <c r="V565" s="2"/>
     </row>
     <row r="566" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A566" s="2"/>
-      <c r="B566" s="2"/>
-      <c r="C566" s="2"/>
-      <c r="D566" s="2"/>
+      <c r="A566" s="2" t="s">
+        <v>590</v>
+      </c>
+      <c r="B566" s="2" t="s">
+        <v>988</v>
+      </c>
+      <c r="C566" s="2">
+        <v>2740</v>
+      </c>
+      <c r="D566" s="2">
+        <v>741</v>
+      </c>
       <c r="E566" s="2" t="s">
         <v>590</v>
       </c>
@@ -28725,10 +29423,18 @@
       <c r="V600" s="2"/>
     </row>
     <row r="601" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A601" s="2"/>
-      <c r="B601" s="2"/>
-      <c r="C601" s="2"/>
-      <c r="D601" s="2"/>
+      <c r="A601" s="2" t="s">
+        <v>948</v>
+      </c>
+      <c r="B601" s="2" t="s">
+        <v>949</v>
+      </c>
+      <c r="C601" s="2">
+        <v>2911</v>
+      </c>
+      <c r="D601" s="2">
+        <v>302</v>
+      </c>
       <c r="E601" s="2" t="s">
         <v>625</v>
       </c>
@@ -32154,10 +32860,18 @@
       <c r="V681" s="2"/>
     </row>
     <row r="682" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A682" s="2"/>
-      <c r="B682" s="2"/>
-      <c r="C682" s="2"/>
-      <c r="D682" s="2"/>
+      <c r="A682" s="2" t="s">
+        <v>946</v>
+      </c>
+      <c r="B682" s="2" t="s">
+        <v>947</v>
+      </c>
+      <c r="C682" s="2">
+        <v>2274</v>
+      </c>
+      <c r="D682" s="2">
+        <v>199</v>
+      </c>
       <c r="E682" s="2" t="s">
         <v>706</v>
       </c>
@@ -34169,10 +34883,18 @@
       <c r="V728" s="2"/>
     </row>
     <row r="729" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A729" s="2"/>
-      <c r="B729" s="2"/>
-      <c r="C729" s="2"/>
-      <c r="D729" s="2"/>
+      <c r="A729" s="2" t="s">
+        <v>904</v>
+      </c>
+      <c r="B729" s="2" t="s">
+        <v>905</v>
+      </c>
+      <c r="C729" s="2">
+        <v>2796</v>
+      </c>
+      <c r="D729" s="2">
+        <v>739</v>
+      </c>
       <c r="E729" s="2" t="s">
         <v>753</v>
       </c>

</xml_diff>